<commit_message>
Update files and rename search_results.html to index.html
</commit_message>
<xml_diff>
--- a/数据表1.xlsx
+++ b/数据表1.xlsx
@@ -7,10 +7,10 @@
     <workbookView windowWidth="28800" windowHeight="12375"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$H$282</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$282</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1889,7 +1889,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -2014,7 +2014,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -2022,6 +2022,9 @@
         <v>0.745138888888889</v>
       </c>
       <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11">
         <v>6</v>
       </c>
     </row>

</xml_diff>